<commit_message>
Update estadisticas tinka 1
</commit_message>
<xml_diff>
--- a/datasets/rgomez/Estadistica Tinka.xlsx
+++ b/datasets/rgomez/Estadistica Tinka.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comercial_01\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael\Documents\GitHub\python-ml-course\datasets\rgomez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C26B05-D553-4DB0-A66A-8C748828BA77}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja5" sheetId="5" r:id="rId3"/>
-    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Ordenados" sheetId="4" r:id="rId4"/>
+    <sheet name="Media" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Media!$A$1:$AE$1</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,15 +36,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>2018-1994</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Sumatoria</t>
+  </si>
+  <si>
+    <t>Desviacion Estandar</t>
+  </si>
+  <si>
+    <t>Numero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -511,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -697,6 +712,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,11 +1006,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:AZ1048576"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8273,11 +8297,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AZ1" sqref="C1:AZ1048576"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15682,11 +15706,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C9EB6F-3A08-46B5-9C65-95A33A201EA7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H71" sqref="H27:H71"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F52" sqref="A31:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16469,10 +16493,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254C76AD-D106-4111-AF3D-839A0B53CB04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -20434,4 +20458,4532 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="31" max="31" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="80">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="80">
+        <v>2019</v>
+      </c>
+      <c r="D1" s="80">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="78">
+        <v>2017</v>
+      </c>
+      <c r="F1" s="78">
+        <v>2016</v>
+      </c>
+      <c r="G1" s="78">
+        <v>2015</v>
+      </c>
+      <c r="H1" s="78">
+        <v>2014</v>
+      </c>
+      <c r="I1" s="78">
+        <v>2013</v>
+      </c>
+      <c r="J1" s="78">
+        <v>2012</v>
+      </c>
+      <c r="K1" s="78">
+        <v>2011</v>
+      </c>
+      <c r="L1" s="78">
+        <v>2010</v>
+      </c>
+      <c r="M1" s="78">
+        <v>2009</v>
+      </c>
+      <c r="N1" s="78">
+        <v>2008</v>
+      </c>
+      <c r="O1" s="78">
+        <v>2007</v>
+      </c>
+      <c r="P1" s="78">
+        <v>2006</v>
+      </c>
+      <c r="Q1" s="78">
+        <v>2005</v>
+      </c>
+      <c r="R1" s="78">
+        <v>2004</v>
+      </c>
+      <c r="S1" s="78">
+        <v>2003</v>
+      </c>
+      <c r="T1" s="78">
+        <v>2002</v>
+      </c>
+      <c r="U1" s="78">
+        <v>2001</v>
+      </c>
+      <c r="V1" s="78">
+        <v>2000</v>
+      </c>
+      <c r="W1" s="78">
+        <v>1999</v>
+      </c>
+      <c r="X1" s="78">
+        <v>1998</v>
+      </c>
+      <c r="Y1" s="78">
+        <v>1997</v>
+      </c>
+      <c r="Z1" s="78">
+        <v>1996</v>
+      </c>
+      <c r="AA1" s="78">
+        <v>1995</v>
+      </c>
+      <c r="AB1" s="78">
+        <v>1994</v>
+      </c>
+      <c r="AC1" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD1" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31">
+        <v>17</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10">
+        <v>15</v>
+      </c>
+      <c r="D2" s="10">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9">
+        <v>13</v>
+      </c>
+      <c r="F2" s="9">
+        <v>14</v>
+      </c>
+      <c r="G2" s="9">
+        <v>13</v>
+      </c>
+      <c r="H2" s="9">
+        <v>14</v>
+      </c>
+      <c r="I2" s="9">
+        <v>15</v>
+      </c>
+      <c r="J2" s="9">
+        <v>14</v>
+      </c>
+      <c r="K2" s="9">
+        <v>9</v>
+      </c>
+      <c r="L2" s="9">
+        <v>14</v>
+      </c>
+      <c r="M2" s="9">
+        <v>13</v>
+      </c>
+      <c r="N2" s="9">
+        <v>15</v>
+      </c>
+      <c r="O2" s="9">
+        <v>8</v>
+      </c>
+      <c r="P2" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>13</v>
+      </c>
+      <c r="R2" s="9">
+        <v>10</v>
+      </c>
+      <c r="S2" s="9">
+        <v>8</v>
+      </c>
+      <c r="T2" s="9">
+        <v>16</v>
+      </c>
+      <c r="U2" s="9">
+        <v>6</v>
+      </c>
+      <c r="V2" s="9">
+        <v>10</v>
+      </c>
+      <c r="W2" s="9">
+        <v>11</v>
+      </c>
+      <c r="X2" s="9">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="9">
+        <v>9</v>
+      </c>
+      <c r="Z2" s="9">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="9">
+        <f>SUM(B2:AB2)</f>
+        <v>287</v>
+      </c>
+      <c r="AD2" s="9">
+        <f>SUM(B2:AB2)/27</f>
+        <v>10.62962962962963</v>
+      </c>
+      <c r="AE2" s="9">
+        <f>_xlfn.STDEV.S(B2:AB2)</f>
+        <v>4.0301569748789232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1">
+        <v>12</v>
+      </c>
+      <c r="M3" s="1">
+        <v>11</v>
+      </c>
+      <c r="N3" s="1">
+        <v>10</v>
+      </c>
+      <c r="O3" s="1">
+        <v>7</v>
+      </c>
+      <c r="P3" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>12</v>
+      </c>
+      <c r="R3" s="1">
+        <v>9</v>
+      </c>
+      <c r="S3" s="1">
+        <v>6</v>
+      </c>
+      <c r="T3" s="1">
+        <v>11</v>
+      </c>
+      <c r="U3" s="1">
+        <v>9</v>
+      </c>
+      <c r="V3" s="1">
+        <v>9</v>
+      </c>
+      <c r="W3" s="1">
+        <v>4</v>
+      </c>
+      <c r="X3" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>12</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC3" s="1">
+        <f>SUM(B3:AB3)</f>
+        <v>283</v>
+      </c>
+      <c r="AD3" s="9">
+        <f>SUM(B3:AB3)/27</f>
+        <v>10.481481481481481</v>
+      </c>
+      <c r="AE3" s="9">
+        <f>_xlfn.STDEV.S(B3:AB3)</f>
+        <v>4.2459969416486905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1">
+        <v>11</v>
+      </c>
+      <c r="K4" s="1">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1">
+        <v>20</v>
+      </c>
+      <c r="M4" s="1">
+        <v>17</v>
+      </c>
+      <c r="N4" s="1">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1">
+        <v>9</v>
+      </c>
+      <c r="P4" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>18</v>
+      </c>
+      <c r="R4" s="1">
+        <v>8</v>
+      </c>
+      <c r="S4" s="1">
+        <v>9</v>
+      </c>
+      <c r="T4" s="1">
+        <v>9</v>
+      </c>
+      <c r="U4" s="1">
+        <v>6</v>
+      </c>
+      <c r="V4" s="1">
+        <v>11</v>
+      </c>
+      <c r="W4" s="1">
+        <v>7</v>
+      </c>
+      <c r="X4" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC4" s="1">
+        <f>SUM(B4:AB4)</f>
+        <v>282</v>
+      </c>
+      <c r="AD4" s="9">
+        <f>SUM(B4:AB4)/27</f>
+        <v>10.444444444444445</v>
+      </c>
+      <c r="AE4" s="9">
+        <f>_xlfn.STDEV.S(B4:AB4)</f>
+        <v>4.3175254071082936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1">
+        <v>21</v>
+      </c>
+      <c r="I5" s="1">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1">
+        <v>11</v>
+      </c>
+      <c r="K5" s="1">
+        <v>12</v>
+      </c>
+      <c r="L5" s="1">
+        <v>13</v>
+      </c>
+      <c r="M5" s="1">
+        <v>17</v>
+      </c>
+      <c r="N5" s="1">
+        <v>14</v>
+      </c>
+      <c r="O5" s="1">
+        <v>10</v>
+      </c>
+      <c r="P5" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>9</v>
+      </c>
+      <c r="R5" s="1">
+        <v>15</v>
+      </c>
+      <c r="S5" s="1">
+        <v>10</v>
+      </c>
+      <c r="T5" s="1">
+        <v>9</v>
+      </c>
+      <c r="U5" s="1">
+        <v>10</v>
+      </c>
+      <c r="V5" s="1">
+        <v>5</v>
+      </c>
+      <c r="W5" s="1">
+        <v>12</v>
+      </c>
+      <c r="X5" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>14</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="1">
+        <f>SUM(B5:AB5)</f>
+        <v>302</v>
+      </c>
+      <c r="AD5" s="9">
+        <f>SUM(B5:AB5)/27</f>
+        <v>11.185185185185185</v>
+      </c>
+      <c r="AE5" s="9">
+        <f>_xlfn.STDEV.S(B5:AB5)</f>
+        <v>4.3680398441145281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1">
+        <v>11</v>
+      </c>
+      <c r="K6" s="1">
+        <v>17</v>
+      </c>
+      <c r="L6" s="1">
+        <v>17</v>
+      </c>
+      <c r="M6" s="1">
+        <v>10</v>
+      </c>
+      <c r="N6" s="1">
+        <v>15</v>
+      </c>
+      <c r="O6" s="1">
+        <v>12</v>
+      </c>
+      <c r="P6" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>9</v>
+      </c>
+      <c r="R6" s="1">
+        <v>8</v>
+      </c>
+      <c r="S6" s="1">
+        <v>5</v>
+      </c>
+      <c r="T6" s="1">
+        <v>4</v>
+      </c>
+      <c r="U6" s="1">
+        <v>10</v>
+      </c>
+      <c r="V6" s="1">
+        <v>7</v>
+      </c>
+      <c r="W6" s="1">
+        <v>10</v>
+      </c>
+      <c r="X6" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>8</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="1">
+        <f>SUM(B6:AB6)</f>
+        <v>260</v>
+      </c>
+      <c r="AD6" s="9">
+        <f>SUM(B6:AB6)/27</f>
+        <v>9.6296296296296298</v>
+      </c>
+      <c r="AE6" s="9">
+        <f>_xlfn.STDEV.S(B6:AB6)</f>
+        <v>4.3865892493103606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>11</v>
+      </c>
+      <c r="I7" s="1">
+        <v>17</v>
+      </c>
+      <c r="J7" s="1">
+        <v>17</v>
+      </c>
+      <c r="K7" s="1">
+        <v>12</v>
+      </c>
+      <c r="L7" s="1">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1">
+        <v>14</v>
+      </c>
+      <c r="N7" s="1">
+        <v>9</v>
+      </c>
+      <c r="O7" s="1">
+        <v>10</v>
+      </c>
+      <c r="P7" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>14</v>
+      </c>
+      <c r="R7" s="1">
+        <v>8</v>
+      </c>
+      <c r="S7" s="1">
+        <v>7</v>
+      </c>
+      <c r="T7" s="1">
+        <v>5</v>
+      </c>
+      <c r="U7" s="1">
+        <v>5</v>
+      </c>
+      <c r="V7" s="1">
+        <v>4</v>
+      </c>
+      <c r="W7" s="1">
+        <v>10</v>
+      </c>
+      <c r="X7" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>16</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="1">
+        <f>SUM(B7:AB7)</f>
+        <v>262</v>
+      </c>
+      <c r="AD7" s="9">
+        <f>SUM(B7:AB7)/27</f>
+        <v>9.7037037037037042</v>
+      </c>
+      <c r="AE7" s="9">
+        <f>_xlfn.STDEV.S(B7:AB7)</f>
+        <v>4.6394198478060291</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24">
+        <v>30</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8">
+        <v>10</v>
+      </c>
+      <c r="D8" s="8">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7">
+        <v>14</v>
+      </c>
+      <c r="G8" s="7">
+        <v>15</v>
+      </c>
+      <c r="H8" s="7">
+        <v>18</v>
+      </c>
+      <c r="I8" s="7">
+        <v>13</v>
+      </c>
+      <c r="J8" s="7">
+        <v>16</v>
+      </c>
+      <c r="K8" s="7">
+        <v>7</v>
+      </c>
+      <c r="L8" s="7">
+        <v>13</v>
+      </c>
+      <c r="M8" s="7">
+        <v>13</v>
+      </c>
+      <c r="N8" s="7">
+        <v>19</v>
+      </c>
+      <c r="O8" s="7">
+        <v>15</v>
+      </c>
+      <c r="P8" s="7">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>11</v>
+      </c>
+      <c r="R8" s="7">
+        <v>14</v>
+      </c>
+      <c r="S8" s="7">
+        <v>11</v>
+      </c>
+      <c r="T8" s="7">
+        <v>3</v>
+      </c>
+      <c r="U8" s="7">
+        <v>10</v>
+      </c>
+      <c r="V8" s="7">
+        <v>7</v>
+      </c>
+      <c r="W8" s="7">
+        <v>8</v>
+      </c>
+      <c r="X8" s="7">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="7">
+        <v>11</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AB8" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC8" s="7">
+        <f>SUM(B8:AB8)</f>
+        <v>292</v>
+      </c>
+      <c r="AD8" s="9">
+        <f>SUM(B8:AB8)/27</f>
+        <v>10.814814814814815</v>
+      </c>
+      <c r="AE8" s="9">
+        <f>_xlfn.STDEV.S(B8:AB8)</f>
+        <v>4.6742916948991153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1">
+        <v>18</v>
+      </c>
+      <c r="K9" s="1">
+        <v>8</v>
+      </c>
+      <c r="L9" s="1">
+        <v>19</v>
+      </c>
+      <c r="M9" s="1">
+        <v>14</v>
+      </c>
+      <c r="N9" s="1">
+        <v>11</v>
+      </c>
+      <c r="O9" s="1">
+        <v>17</v>
+      </c>
+      <c r="P9" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>13</v>
+      </c>
+      <c r="R9" s="1">
+        <v>9</v>
+      </c>
+      <c r="S9" s="1">
+        <v>11</v>
+      </c>
+      <c r="T9" s="1">
+        <v>8</v>
+      </c>
+      <c r="U9" s="1">
+        <v>5</v>
+      </c>
+      <c r="V9" s="1">
+        <v>4</v>
+      </c>
+      <c r="W9" s="1">
+        <v>6</v>
+      </c>
+      <c r="X9" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>11</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="1">
+        <f>SUM(B9:AB9)</f>
+        <v>265</v>
+      </c>
+      <c r="AD9" s="9">
+        <f>SUM(B9:AB9)/27</f>
+        <v>9.8148148148148149</v>
+      </c>
+      <c r="AE9" s="9">
+        <f>_xlfn.STDEV.S(B9:AB9)</f>
+        <v>4.7070898819435296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1">
+        <v>16</v>
+      </c>
+      <c r="H10" s="1">
+        <v>15</v>
+      </c>
+      <c r="I10" s="1">
+        <v>14</v>
+      </c>
+      <c r="J10" s="1">
+        <v>14</v>
+      </c>
+      <c r="K10" s="1">
+        <v>11</v>
+      </c>
+      <c r="L10" s="1">
+        <v>11</v>
+      </c>
+      <c r="M10" s="1">
+        <v>11</v>
+      </c>
+      <c r="N10" s="1">
+        <v>10</v>
+      </c>
+      <c r="O10" s="1">
+        <v>12</v>
+      </c>
+      <c r="P10" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>11</v>
+      </c>
+      <c r="R10" s="1">
+        <v>17</v>
+      </c>
+      <c r="S10" s="1">
+        <v>8</v>
+      </c>
+      <c r="T10" s="1">
+        <v>7</v>
+      </c>
+      <c r="U10" s="1">
+        <v>8</v>
+      </c>
+      <c r="V10" s="1">
+        <v>2</v>
+      </c>
+      <c r="W10" s="1">
+        <v>9</v>
+      </c>
+      <c r="X10" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <f>SUM(B10:AB10)</f>
+        <v>274</v>
+      </c>
+      <c r="AD10" s="9">
+        <f>SUM(B10:AB10)/27</f>
+        <v>10.148148148148149</v>
+      </c>
+      <c r="AE10" s="9">
+        <f>_xlfn.STDEV.S(B10:AB10)</f>
+        <v>4.720688539281138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1">
+        <v>12</v>
+      </c>
+      <c r="H11" s="1">
+        <v>18</v>
+      </c>
+      <c r="I11" s="1">
+        <v>16</v>
+      </c>
+      <c r="J11" s="1">
+        <v>14</v>
+      </c>
+      <c r="K11" s="1">
+        <v>10</v>
+      </c>
+      <c r="L11" s="1">
+        <v>15</v>
+      </c>
+      <c r="M11" s="1">
+        <v>12</v>
+      </c>
+      <c r="N11" s="1">
+        <v>12</v>
+      </c>
+      <c r="O11" s="1">
+        <v>17</v>
+      </c>
+      <c r="P11" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>13</v>
+      </c>
+      <c r="R11" s="1">
+        <v>11</v>
+      </c>
+      <c r="S11" s="1">
+        <v>3</v>
+      </c>
+      <c r="T11" s="1">
+        <v>8</v>
+      </c>
+      <c r="U11" s="1">
+        <v>9</v>
+      </c>
+      <c r="V11" s="1">
+        <v>10</v>
+      </c>
+      <c r="W11" s="1">
+        <v>7</v>
+      </c>
+      <c r="X11" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="1">
+        <f>SUM(B11:AB11)</f>
+        <v>285</v>
+      </c>
+      <c r="AD11" s="9">
+        <f>SUM(B11:AB11)/27</f>
+        <v>10.555555555555555</v>
+      </c>
+      <c r="AE11" s="9">
+        <f>_xlfn.STDEV.S(B11:AB11)</f>
+        <v>4.7258156262526079</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1">
+        <v>16</v>
+      </c>
+      <c r="H12" s="1">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1">
+        <v>11</v>
+      </c>
+      <c r="J12" s="1">
+        <v>14</v>
+      </c>
+      <c r="K12" s="1">
+        <v>9</v>
+      </c>
+      <c r="L12" s="1">
+        <v>15</v>
+      </c>
+      <c r="M12" s="1">
+        <v>18</v>
+      </c>
+      <c r="N12" s="1">
+        <v>8</v>
+      </c>
+      <c r="O12" s="1">
+        <v>19</v>
+      </c>
+      <c r="P12" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>15</v>
+      </c>
+      <c r="R12" s="1">
+        <v>11</v>
+      </c>
+      <c r="S12" s="1">
+        <v>4</v>
+      </c>
+      <c r="T12" s="1">
+        <v>7</v>
+      </c>
+      <c r="U12" s="1">
+        <v>7</v>
+      </c>
+      <c r="V12" s="1">
+        <v>8</v>
+      </c>
+      <c r="W12" s="1">
+        <v>6</v>
+      </c>
+      <c r="X12" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>13</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="1">
+        <f>SUM(B12:AB12)</f>
+        <v>286</v>
+      </c>
+      <c r="AD12" s="9">
+        <f>SUM(B12:AB12)/27</f>
+        <v>10.592592592592593</v>
+      </c>
+      <c r="AE12" s="9">
+        <f>_xlfn.STDEV.S(B12:AB12)</f>
+        <v>4.733345371358233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1">
+        <v>16</v>
+      </c>
+      <c r="H13" s="1">
+        <v>11</v>
+      </c>
+      <c r="I13" s="1">
+        <v>12</v>
+      </c>
+      <c r="J13" s="1">
+        <v>16</v>
+      </c>
+      <c r="K13" s="1">
+        <v>9</v>
+      </c>
+      <c r="L13" s="1">
+        <v>8</v>
+      </c>
+      <c r="M13" s="1">
+        <v>11</v>
+      </c>
+      <c r="N13" s="1">
+        <v>15</v>
+      </c>
+      <c r="O13" s="1">
+        <v>13</v>
+      </c>
+      <c r="P13" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>14</v>
+      </c>
+      <c r="R13" s="1">
+        <v>12</v>
+      </c>
+      <c r="S13" s="1">
+        <v>4</v>
+      </c>
+      <c r="T13" s="1">
+        <v>4</v>
+      </c>
+      <c r="U13" s="1">
+        <v>4</v>
+      </c>
+      <c r="V13" s="1">
+        <v>7</v>
+      </c>
+      <c r="W13" s="1">
+        <v>2</v>
+      </c>
+      <c r="X13" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="1">
+        <f>SUM(B13:AB13)</f>
+        <v>241</v>
+      </c>
+      <c r="AD13" s="9">
+        <f>SUM(B13:AB13)/27</f>
+        <v>8.9259259259259256</v>
+      </c>
+      <c r="AE13" s="9">
+        <f>_xlfn.STDEV.S(B13:AB13)</f>
+        <v>4.7549644172892194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>14</v>
+      </c>
+      <c r="D14" s="2">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1">
+        <v>17</v>
+      </c>
+      <c r="G14" s="1">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1">
+        <v>17</v>
+      </c>
+      <c r="I14" s="1">
+        <v>16</v>
+      </c>
+      <c r="J14" s="1">
+        <v>18</v>
+      </c>
+      <c r="K14" s="1">
+        <v>13</v>
+      </c>
+      <c r="L14" s="1">
+        <v>15</v>
+      </c>
+      <c r="M14" s="1">
+        <v>15</v>
+      </c>
+      <c r="N14" s="1">
+        <v>11</v>
+      </c>
+      <c r="O14" s="1">
+        <v>12</v>
+      </c>
+      <c r="P14" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>13</v>
+      </c>
+      <c r="R14" s="1">
+        <v>10</v>
+      </c>
+      <c r="S14" s="1">
+        <v>6</v>
+      </c>
+      <c r="T14" s="1">
+        <v>10</v>
+      </c>
+      <c r="U14" s="1">
+        <v>3</v>
+      </c>
+      <c r="V14" s="1">
+        <v>5</v>
+      </c>
+      <c r="W14" s="1">
+        <v>13</v>
+      </c>
+      <c r="X14" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC14" s="1">
+        <f>SUM(B14:AB14)</f>
+        <v>285</v>
+      </c>
+      <c r="AD14" s="9">
+        <f>SUM(B14:AB14)/27</f>
+        <v>10.555555555555555</v>
+      </c>
+      <c r="AE14" s="9">
+        <f>_xlfn.STDEV.S(B14:AB14)</f>
+        <v>4.7663349355609403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1">
+        <v>16</v>
+      </c>
+      <c r="H15" s="1">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1">
+        <v>12</v>
+      </c>
+      <c r="J15" s="1">
+        <v>12</v>
+      </c>
+      <c r="K15" s="1">
+        <v>16</v>
+      </c>
+      <c r="L15" s="1">
+        <v>7</v>
+      </c>
+      <c r="M15" s="1">
+        <v>11</v>
+      </c>
+      <c r="N15" s="1">
+        <v>15</v>
+      </c>
+      <c r="O15" s="1">
+        <v>11</v>
+      </c>
+      <c r="P15" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>13</v>
+      </c>
+      <c r="R15" s="1">
+        <v>11</v>
+      </c>
+      <c r="S15" s="1">
+        <v>8</v>
+      </c>
+      <c r="T15" s="1">
+        <v>9</v>
+      </c>
+      <c r="U15" s="1">
+        <v>6</v>
+      </c>
+      <c r="V15" s="1">
+        <v>4</v>
+      </c>
+      <c r="W15" s="1">
+        <v>5</v>
+      </c>
+      <c r="X15" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC15" s="1">
+        <f>SUM(B15:AB15)</f>
+        <v>276</v>
+      </c>
+      <c r="AD15" s="9">
+        <f>SUM(B15:AB15)/27</f>
+        <v>10.222222222222221</v>
+      </c>
+      <c r="AE15" s="9">
+        <f>_xlfn.STDEV.S(B15:AB15)</f>
+        <v>4.782446536219183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1">
+        <v>11</v>
+      </c>
+      <c r="G16" s="1">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1">
+        <v>11</v>
+      </c>
+      <c r="I16" s="1">
+        <v>11</v>
+      </c>
+      <c r="J16" s="1">
+        <v>13</v>
+      </c>
+      <c r="K16" s="1">
+        <v>13</v>
+      </c>
+      <c r="L16" s="1">
+        <v>11</v>
+      </c>
+      <c r="M16" s="1">
+        <v>13</v>
+      </c>
+      <c r="N16" s="1">
+        <v>14</v>
+      </c>
+      <c r="O16" s="1">
+        <v>14</v>
+      </c>
+      <c r="P16" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>8</v>
+      </c>
+      <c r="R16" s="1">
+        <v>13</v>
+      </c>
+      <c r="S16" s="1">
+        <v>4</v>
+      </c>
+      <c r="T16" s="1">
+        <v>8</v>
+      </c>
+      <c r="U16" s="1">
+        <v>8</v>
+      </c>
+      <c r="V16" s="1">
+        <v>5</v>
+      </c>
+      <c r="W16" s="1">
+        <v>8</v>
+      </c>
+      <c r="X16" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1">
+        <f>SUM(B16:AB16)</f>
+        <v>232</v>
+      </c>
+      <c r="AD16" s="9">
+        <f>SUM(B16:AB16)/27</f>
+        <v>8.5925925925925934</v>
+      </c>
+      <c r="AE16" s="9">
+        <f>_xlfn.STDEV.S(B16:AB16)</f>
+        <v>4.7979102763539689</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1">
+        <v>7</v>
+      </c>
+      <c r="H17" s="1">
+        <v>15</v>
+      </c>
+      <c r="I17" s="1">
+        <v>13</v>
+      </c>
+      <c r="J17" s="1">
+        <v>18</v>
+      </c>
+      <c r="K17" s="1">
+        <v>17</v>
+      </c>
+      <c r="L17" s="1">
+        <v>10</v>
+      </c>
+      <c r="M17" s="1">
+        <v>13</v>
+      </c>
+      <c r="N17" s="1">
+        <v>15</v>
+      </c>
+      <c r="O17" s="1">
+        <v>14</v>
+      </c>
+      <c r="P17" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>20</v>
+      </c>
+      <c r="R17" s="1">
+        <v>15</v>
+      </c>
+      <c r="S17" s="1">
+        <v>7</v>
+      </c>
+      <c r="T17" s="1">
+        <v>8</v>
+      </c>
+      <c r="U17" s="1">
+        <v>7</v>
+      </c>
+      <c r="V17" s="1">
+        <v>5</v>
+      </c>
+      <c r="W17" s="1">
+        <v>11</v>
+      </c>
+      <c r="X17" s="1">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>11</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="1">
+        <f>SUM(B17:AB17)</f>
+        <v>312</v>
+      </c>
+      <c r="AD17" s="9">
+        <f>SUM(B17:AB17)/27</f>
+        <v>11.555555555555555</v>
+      </c>
+      <c r="AE17" s="9">
+        <f>_xlfn.STDEV.S(B17:AB17)</f>
+        <v>4.8304589153964788</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1">
+        <v>18</v>
+      </c>
+      <c r="G18" s="1">
+        <v>15</v>
+      </c>
+      <c r="H18" s="1">
+        <v>12</v>
+      </c>
+      <c r="I18" s="1">
+        <v>19</v>
+      </c>
+      <c r="J18" s="1">
+        <v>17</v>
+      </c>
+      <c r="K18" s="1">
+        <v>10</v>
+      </c>
+      <c r="L18" s="1">
+        <v>11</v>
+      </c>
+      <c r="M18" s="1">
+        <v>11</v>
+      </c>
+      <c r="N18" s="1">
+        <v>17</v>
+      </c>
+      <c r="O18" s="1">
+        <v>11</v>
+      </c>
+      <c r="P18" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>14</v>
+      </c>
+      <c r="R18" s="1">
+        <v>10</v>
+      </c>
+      <c r="S18" s="1">
+        <v>5</v>
+      </c>
+      <c r="T18" s="1">
+        <v>6</v>
+      </c>
+      <c r="U18" s="1">
+        <v>7</v>
+      </c>
+      <c r="V18" s="1">
+        <v>14</v>
+      </c>
+      <c r="W18" s="1">
+        <v>8</v>
+      </c>
+      <c r="X18" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>12</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>12</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="1">
+        <f>SUM(B18:AB18)</f>
+        <v>301</v>
+      </c>
+      <c r="AD18" s="9">
+        <f>SUM(B18:AB18)/27</f>
+        <v>11.148148148148149</v>
+      </c>
+      <c r="AE18" s="9">
+        <f>_xlfn.STDEV.S(B18:AB18)</f>
+        <v>4.8492957752306172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>11</v>
+      </c>
+      <c r="D19" s="2">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1">
+        <v>13</v>
+      </c>
+      <c r="H19" s="1">
+        <v>16</v>
+      </c>
+      <c r="I19" s="1">
+        <v>10</v>
+      </c>
+      <c r="J19" s="1">
+        <v>11</v>
+      </c>
+      <c r="K19" s="1">
+        <v>18</v>
+      </c>
+      <c r="L19" s="1">
+        <v>16</v>
+      </c>
+      <c r="M19" s="1">
+        <v>10</v>
+      </c>
+      <c r="N19" s="1">
+        <v>17</v>
+      </c>
+      <c r="O19" s="1">
+        <v>22</v>
+      </c>
+      <c r="P19" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>11</v>
+      </c>
+      <c r="R19" s="1">
+        <v>11</v>
+      </c>
+      <c r="S19" s="1">
+        <v>10</v>
+      </c>
+      <c r="T19" s="1">
+        <v>5</v>
+      </c>
+      <c r="U19" s="1">
+        <v>11</v>
+      </c>
+      <c r="V19" s="1">
+        <v>6</v>
+      </c>
+      <c r="W19" s="1">
+        <v>10</v>
+      </c>
+      <c r="X19" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC19" s="1">
+        <f>SUM(B19:AB19)</f>
+        <v>284</v>
+      </c>
+      <c r="AD19" s="9">
+        <f>SUM(B19:AB19)/27</f>
+        <v>10.518518518518519</v>
+      </c>
+      <c r="AE19" s="9">
+        <f>_xlfn.STDEV.S(B19:AB19)</f>
+        <v>4.8545804728062318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1">
+        <v>19</v>
+      </c>
+      <c r="F20" s="1">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1">
+        <v>14</v>
+      </c>
+      <c r="I20" s="1">
+        <v>11</v>
+      </c>
+      <c r="J20" s="1">
+        <v>9</v>
+      </c>
+      <c r="K20" s="1">
+        <v>20</v>
+      </c>
+      <c r="L20" s="1">
+        <v>17</v>
+      </c>
+      <c r="M20" s="1">
+        <v>12</v>
+      </c>
+      <c r="N20" s="1">
+        <v>9</v>
+      </c>
+      <c r="O20" s="1">
+        <v>13</v>
+      </c>
+      <c r="P20" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>8</v>
+      </c>
+      <c r="R20" s="1">
+        <v>8</v>
+      </c>
+      <c r="S20" s="1">
+        <v>6</v>
+      </c>
+      <c r="T20" s="1">
+        <v>7</v>
+      </c>
+      <c r="U20" s="1">
+        <v>9</v>
+      </c>
+      <c r="V20" s="1">
+        <v>9</v>
+      </c>
+      <c r="W20" s="1">
+        <v>7</v>
+      </c>
+      <c r="X20" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="1">
+        <f>SUM(B20:AB20)</f>
+        <v>266</v>
+      </c>
+      <c r="AD20" s="9">
+        <f>SUM(B20:AB20)/27</f>
+        <v>9.8518518518518512</v>
+      </c>
+      <c r="AE20" s="9">
+        <f>_xlfn.STDEV.S(B20:AB20)</f>
+        <v>4.857220665420976</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>13</v>
+      </c>
+      <c r="D21" s="2">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1">
+        <v>14</v>
+      </c>
+      <c r="F21" s="1">
+        <v>15</v>
+      </c>
+      <c r="G21" s="1">
+        <v>14</v>
+      </c>
+      <c r="H21" s="1">
+        <v>16</v>
+      </c>
+      <c r="I21" s="1">
+        <v>14</v>
+      </c>
+      <c r="J21" s="1">
+        <v>16</v>
+      </c>
+      <c r="K21" s="1">
+        <v>16</v>
+      </c>
+      <c r="L21" s="1">
+        <v>16</v>
+      </c>
+      <c r="M21" s="1">
+        <v>13</v>
+      </c>
+      <c r="N21" s="1">
+        <v>15</v>
+      </c>
+      <c r="O21" s="1">
+        <v>18</v>
+      </c>
+      <c r="P21" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>13</v>
+      </c>
+      <c r="R21" s="1">
+        <v>12</v>
+      </c>
+      <c r="S21" s="1">
+        <v>7</v>
+      </c>
+      <c r="T21" s="1">
+        <v>3</v>
+      </c>
+      <c r="U21" s="1">
+        <v>12</v>
+      </c>
+      <c r="V21" s="1">
+        <v>6</v>
+      </c>
+      <c r="W21" s="1">
+        <v>4</v>
+      </c>
+      <c r="X21" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="1">
+        <f>SUM(B21:AB21)</f>
+        <v>287</v>
+      </c>
+      <c r="AD21" s="9">
+        <f>SUM(B21:AB21)/27</f>
+        <v>10.62962962962963</v>
+      </c>
+      <c r="AE21" s="9">
+        <f>_xlfn.STDEV.S(B21:AB21)</f>
+        <v>5.0088241223184387</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1">
+        <v>11</v>
+      </c>
+      <c r="F22" s="1">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
+        <v>15</v>
+      </c>
+      <c r="I22" s="1">
+        <v>9</v>
+      </c>
+      <c r="J22" s="1">
+        <v>7</v>
+      </c>
+      <c r="K22" s="1">
+        <v>15</v>
+      </c>
+      <c r="L22" s="1">
+        <v>16</v>
+      </c>
+      <c r="M22" s="1">
+        <v>15</v>
+      </c>
+      <c r="N22" s="1">
+        <v>13</v>
+      </c>
+      <c r="O22" s="1">
+        <v>15</v>
+      </c>
+      <c r="P22" s="1">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>16</v>
+      </c>
+      <c r="R22" s="1">
+        <v>15</v>
+      </c>
+      <c r="S22" s="1">
+        <v>6</v>
+      </c>
+      <c r="T22" s="1">
+        <v>8</v>
+      </c>
+      <c r="U22" s="1">
+        <v>8</v>
+      </c>
+      <c r="V22" s="1">
+        <v>6</v>
+      </c>
+      <c r="W22" s="1">
+        <v>5</v>
+      </c>
+      <c r="X22" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>8</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC22" s="1">
+        <f>SUM(B22:AB22)</f>
+        <v>288</v>
+      </c>
+      <c r="AD22" s="9">
+        <f>SUM(B22:AB22)/27</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="AE22" s="9">
+        <f>_xlfn.STDEV.S(B22:AB22)</f>
+        <v>5.0914709979608963</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>14</v>
+      </c>
+      <c r="D23" s="2">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1">
+        <v>9</v>
+      </c>
+      <c r="G23" s="1">
+        <v>15</v>
+      </c>
+      <c r="H23" s="1">
+        <v>14</v>
+      </c>
+      <c r="I23" s="1">
+        <v>12</v>
+      </c>
+      <c r="J23" s="1">
+        <v>6</v>
+      </c>
+      <c r="K23" s="1">
+        <v>12</v>
+      </c>
+      <c r="L23" s="1">
+        <v>11</v>
+      </c>
+      <c r="M23" s="1">
+        <v>10</v>
+      </c>
+      <c r="N23" s="1">
+        <v>17</v>
+      </c>
+      <c r="O23" s="1">
+        <v>14</v>
+      </c>
+      <c r="P23" s="1">
+        <v>23</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>19</v>
+      </c>
+      <c r="R23" s="1">
+        <v>10</v>
+      </c>
+      <c r="S23" s="1">
+        <v>6</v>
+      </c>
+      <c r="T23" s="1">
+        <v>6</v>
+      </c>
+      <c r="U23" s="1">
+        <v>4</v>
+      </c>
+      <c r="V23" s="1">
+        <v>8</v>
+      </c>
+      <c r="W23" s="1">
+        <v>6</v>
+      </c>
+      <c r="X23" s="1">
+        <v>13</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC23" s="1">
+        <f>SUM(B23:AB23)</f>
+        <v>287</v>
+      </c>
+      <c r="AD23" s="9">
+        <f>SUM(B23:AB23)/27</f>
+        <v>10.62962962962963</v>
+      </c>
+      <c r="AE23" s="9">
+        <f>_xlfn.STDEV.S(B23:AB23)</f>
+        <v>5.1451855625365415</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2">
+        <v>13</v>
+      </c>
+      <c r="D24" s="2">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1">
+        <v>19</v>
+      </c>
+      <c r="G24" s="1">
+        <v>14</v>
+      </c>
+      <c r="H24" s="1">
+        <v>17</v>
+      </c>
+      <c r="I24" s="1">
+        <v>18</v>
+      </c>
+      <c r="J24" s="1">
+        <v>20</v>
+      </c>
+      <c r="K24" s="1">
+        <v>13</v>
+      </c>
+      <c r="L24" s="1">
+        <v>12</v>
+      </c>
+      <c r="M24" s="1">
+        <v>11</v>
+      </c>
+      <c r="N24" s="1">
+        <v>10</v>
+      </c>
+      <c r="O24" s="1">
+        <v>16</v>
+      </c>
+      <c r="P24" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>18</v>
+      </c>
+      <c r="R24" s="1">
+        <v>9</v>
+      </c>
+      <c r="S24" s="1">
+        <v>6</v>
+      </c>
+      <c r="T24" s="1">
+        <v>7</v>
+      </c>
+      <c r="U24" s="1">
+        <v>4</v>
+      </c>
+      <c r="V24" s="1">
+        <v>8</v>
+      </c>
+      <c r="W24" s="1">
+        <v>8</v>
+      </c>
+      <c r="X24" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1">
+        <f>SUM(B24:AB24)</f>
+        <v>302</v>
+      </c>
+      <c r="AD24" s="9">
+        <f>SUM(B24:AB24)/27</f>
+        <v>11.185185185185185</v>
+      </c>
+      <c r="AE24" s="9">
+        <f>_xlfn.STDEV.S(B24:AB24)</f>
+        <v>5.1816023437738679</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>16</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>15</v>
+      </c>
+      <c r="D25" s="2">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1">
+        <v>14</v>
+      </c>
+      <c r="G25" s="1">
+        <v>10</v>
+      </c>
+      <c r="H25" s="1">
+        <v>15</v>
+      </c>
+      <c r="I25" s="1">
+        <v>10</v>
+      </c>
+      <c r="J25" s="1">
+        <v>9</v>
+      </c>
+      <c r="K25" s="1">
+        <v>13</v>
+      </c>
+      <c r="L25" s="1">
+        <v>11</v>
+      </c>
+      <c r="M25" s="1">
+        <v>22</v>
+      </c>
+      <c r="N25" s="1">
+        <v>17</v>
+      </c>
+      <c r="O25" s="1">
+        <v>18</v>
+      </c>
+      <c r="P25" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>18</v>
+      </c>
+      <c r="R25" s="1">
+        <v>15</v>
+      </c>
+      <c r="S25" s="1">
+        <v>6</v>
+      </c>
+      <c r="T25" s="1">
+        <v>7</v>
+      </c>
+      <c r="U25" s="1">
+        <v>5</v>
+      </c>
+      <c r="V25" s="1">
+        <v>7</v>
+      </c>
+      <c r="W25" s="1">
+        <v>7</v>
+      </c>
+      <c r="X25" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>13</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC25" s="1">
+        <f>SUM(B25:AB25)</f>
+        <v>294</v>
+      </c>
+      <c r="AD25" s="9">
+        <f>SUM(B25:AB25)/27</f>
+        <v>10.888888888888889</v>
+      </c>
+      <c r="AE25" s="9">
+        <f>_xlfn.STDEV.S(B25:AB25)</f>
+        <v>5.1838011991004116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>16</v>
+      </c>
+      <c r="D26" s="2">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1">
+        <v>13</v>
+      </c>
+      <c r="F26" s="1">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1">
+        <v>10</v>
+      </c>
+      <c r="H26" s="1">
+        <v>23</v>
+      </c>
+      <c r="I26" s="1">
+        <v>12</v>
+      </c>
+      <c r="J26" s="1">
+        <v>16</v>
+      </c>
+      <c r="K26" s="1">
+        <v>10</v>
+      </c>
+      <c r="L26" s="1">
+        <v>20</v>
+      </c>
+      <c r="M26" s="1">
+        <v>13</v>
+      </c>
+      <c r="N26" s="1">
+        <v>14</v>
+      </c>
+      <c r="O26" s="1">
+        <v>12</v>
+      </c>
+      <c r="P26" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>15</v>
+      </c>
+      <c r="R26" s="1">
+        <v>10</v>
+      </c>
+      <c r="S26" s="1">
+        <v>4</v>
+      </c>
+      <c r="T26" s="1">
+        <v>6</v>
+      </c>
+      <c r="U26" s="1">
+        <v>5</v>
+      </c>
+      <c r="V26" s="1">
+        <v>8</v>
+      </c>
+      <c r="W26" s="1">
+        <v>8</v>
+      </c>
+      <c r="X26" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC26" s="1">
+        <f>SUM(B26:AB26)</f>
+        <v>287</v>
+      </c>
+      <c r="AD26" s="9">
+        <f>SUM(B26:AB26)/27</f>
+        <v>10.62962962962963</v>
+      </c>
+      <c r="AE26" s="9">
+        <f>_xlfn.STDEV.S(B26:AB26)</f>
+        <v>5.2267665261697225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2">
+        <v>6</v>
+      </c>
+      <c r="E27" s="1">
+        <v>6</v>
+      </c>
+      <c r="F27" s="1">
+        <v>16</v>
+      </c>
+      <c r="G27" s="1">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1">
+        <v>17</v>
+      </c>
+      <c r="I27" s="1">
+        <v>15</v>
+      </c>
+      <c r="J27" s="1">
+        <v>20</v>
+      </c>
+      <c r="K27" s="1">
+        <v>11</v>
+      </c>
+      <c r="L27" s="1">
+        <v>9</v>
+      </c>
+      <c r="M27" s="1">
+        <v>12</v>
+      </c>
+      <c r="N27" s="1">
+        <v>14</v>
+      </c>
+      <c r="O27" s="1">
+        <v>16</v>
+      </c>
+      <c r="P27" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>15</v>
+      </c>
+      <c r="R27" s="1">
+        <v>4</v>
+      </c>
+      <c r="S27" s="1">
+        <v>5</v>
+      </c>
+      <c r="T27" s="1">
+        <v>5</v>
+      </c>
+      <c r="U27" s="1">
+        <v>3</v>
+      </c>
+      <c r="V27" s="1">
+        <v>2</v>
+      </c>
+      <c r="W27" s="1">
+        <v>10</v>
+      </c>
+      <c r="X27" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>11</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="1">
+        <f>SUM(B27:AB27)</f>
+        <v>254</v>
+      </c>
+      <c r="AD27" s="9">
+        <f>SUM(B27:AB27)/27</f>
+        <v>9.4074074074074066</v>
+      </c>
+      <c r="AE27" s="9">
+        <f>_xlfn.STDEV.S(B27:AB27)</f>
+        <v>5.2788348019327973</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>14</v>
+      </c>
+      <c r="D28" s="2">
+        <v>9</v>
+      </c>
+      <c r="E28" s="1">
+        <v>16</v>
+      </c>
+      <c r="F28" s="1">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1">
+        <v>10</v>
+      </c>
+      <c r="I28" s="1">
+        <v>15</v>
+      </c>
+      <c r="J28" s="1">
+        <v>19</v>
+      </c>
+      <c r="K28" s="1">
+        <v>23</v>
+      </c>
+      <c r="L28" s="1">
+        <v>14</v>
+      </c>
+      <c r="M28" s="1">
+        <v>18</v>
+      </c>
+      <c r="N28" s="1">
+        <v>6</v>
+      </c>
+      <c r="O28" s="1">
+        <v>16</v>
+      </c>
+      <c r="P28" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>14</v>
+      </c>
+      <c r="R28" s="1">
+        <v>8</v>
+      </c>
+      <c r="S28" s="1">
+        <v>7</v>
+      </c>
+      <c r="T28" s="1">
+        <v>3</v>
+      </c>
+      <c r="U28" s="1">
+        <v>7</v>
+      </c>
+      <c r="V28" s="1">
+        <v>5</v>
+      </c>
+      <c r="W28" s="1">
+        <v>7</v>
+      </c>
+      <c r="X28" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>11</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="1">
+        <f>SUM(B28:AB28)</f>
+        <v>294</v>
+      </c>
+      <c r="AD28" s="9">
+        <f>SUM(B28:AB28)/27</f>
+        <v>10.888888888888889</v>
+      </c>
+      <c r="AE28" s="9">
+        <f>_xlfn.STDEV.S(B28:AB28)</f>
+        <v>5.3156758983604568</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>20</v>
+      </c>
+      <c r="D29" s="2">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1">
+        <v>16</v>
+      </c>
+      <c r="F29" s="1">
+        <v>17</v>
+      </c>
+      <c r="G29" s="1">
+        <v>15</v>
+      </c>
+      <c r="H29" s="1">
+        <v>11</v>
+      </c>
+      <c r="I29" s="1">
+        <v>13</v>
+      </c>
+      <c r="J29" s="1">
+        <v>20</v>
+      </c>
+      <c r="K29" s="1">
+        <v>10</v>
+      </c>
+      <c r="L29" s="1">
+        <v>13</v>
+      </c>
+      <c r="M29" s="1">
+        <v>13</v>
+      </c>
+      <c r="N29" s="1">
+        <v>13</v>
+      </c>
+      <c r="O29" s="1">
+        <v>20</v>
+      </c>
+      <c r="P29" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>14</v>
+      </c>
+      <c r="R29" s="1">
+        <v>6</v>
+      </c>
+      <c r="S29" s="1">
+        <v>5</v>
+      </c>
+      <c r="T29" s="1">
+        <v>7</v>
+      </c>
+      <c r="U29" s="1">
+        <v>7</v>
+      </c>
+      <c r="V29" s="1">
+        <v>7</v>
+      </c>
+      <c r="W29" s="1">
+        <v>5</v>
+      </c>
+      <c r="X29" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="1">
+        <f>SUM(B29:AB29)</f>
+        <v>291</v>
+      </c>
+      <c r="AD29" s="9">
+        <f>SUM(B29:AB29)/27</f>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="AE29" s="9">
+        <f>_xlfn.STDEV.S(B29:AB29)</f>
+        <v>5.3517310882578579</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>11</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1">
+        <v>18</v>
+      </c>
+      <c r="F30" s="1">
+        <v>9</v>
+      </c>
+      <c r="G30" s="1">
+        <v>19</v>
+      </c>
+      <c r="H30" s="1">
+        <v>15</v>
+      </c>
+      <c r="I30" s="1">
+        <v>10</v>
+      </c>
+      <c r="J30" s="1">
+        <v>18</v>
+      </c>
+      <c r="K30" s="1">
+        <v>15</v>
+      </c>
+      <c r="L30" s="1">
+        <v>15</v>
+      </c>
+      <c r="M30" s="1">
+        <v>12</v>
+      </c>
+      <c r="N30" s="1">
+        <v>16</v>
+      </c>
+      <c r="O30" s="1">
+        <v>10</v>
+      </c>
+      <c r="P30" s="1">
+        <v>21</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>11</v>
+      </c>
+      <c r="R30" s="1">
+        <v>14</v>
+      </c>
+      <c r="S30" s="1">
+        <v>7</v>
+      </c>
+      <c r="T30" s="1">
+        <v>4</v>
+      </c>
+      <c r="U30" s="1">
+        <v>6</v>
+      </c>
+      <c r="V30" s="1">
+        <v>5</v>
+      </c>
+      <c r="W30" s="1">
+        <v>6</v>
+      </c>
+      <c r="X30" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y30" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z30" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>16</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="1">
+        <f>SUM(B30:AB30)</f>
+        <v>293</v>
+      </c>
+      <c r="AD30" s="9">
+        <f>SUM(B30:AB30)/27</f>
+        <v>10.851851851851851</v>
+      </c>
+      <c r="AE30" s="9">
+        <f>_xlfn.STDEV.S(B30:AB30)</f>
+        <v>5.3973191614962079</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15">
+        <v>28</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>18</v>
+      </c>
+      <c r="D31" s="2">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1">
+        <v>8</v>
+      </c>
+      <c r="F31" s="1">
+        <v>12</v>
+      </c>
+      <c r="G31" s="1">
+        <v>13</v>
+      </c>
+      <c r="H31" s="1">
+        <v>11</v>
+      </c>
+      <c r="I31" s="1">
+        <v>14</v>
+      </c>
+      <c r="J31" s="1">
+        <v>13</v>
+      </c>
+      <c r="K31" s="1">
+        <v>20</v>
+      </c>
+      <c r="L31" s="1">
+        <v>18</v>
+      </c>
+      <c r="M31" s="1">
+        <v>20</v>
+      </c>
+      <c r="N31" s="1">
+        <v>17</v>
+      </c>
+      <c r="O31" s="1">
+        <v>13</v>
+      </c>
+      <c r="P31" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>10</v>
+      </c>
+      <c r="R31" s="1">
+        <v>16</v>
+      </c>
+      <c r="S31" s="1">
+        <v>9</v>
+      </c>
+      <c r="T31" s="1">
+        <v>3</v>
+      </c>
+      <c r="U31" s="1">
+        <v>7</v>
+      </c>
+      <c r="V31" s="1">
+        <v>10</v>
+      </c>
+      <c r="W31" s="1">
+        <v>8</v>
+      </c>
+      <c r="X31" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="1">
+        <f>SUM(B31:AB31)</f>
+        <v>293</v>
+      </c>
+      <c r="AD31" s="9">
+        <f>SUM(B31:AB31)/27</f>
+        <v>10.851851851851851</v>
+      </c>
+      <c r="AE31" s="9">
+        <f>_xlfn.STDEV.S(B31:AB31)</f>
+        <v>5.4115524837979985</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
+        <v>10</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>15</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1">
+        <v>13</v>
+      </c>
+      <c r="F32" s="1">
+        <v>13</v>
+      </c>
+      <c r="G32" s="1">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1">
+        <v>13</v>
+      </c>
+      <c r="I32" s="1">
+        <v>14</v>
+      </c>
+      <c r="J32" s="1">
+        <v>8</v>
+      </c>
+      <c r="K32" s="1">
+        <v>18</v>
+      </c>
+      <c r="L32" s="1">
+        <v>17</v>
+      </c>
+      <c r="M32" s="1">
+        <v>9</v>
+      </c>
+      <c r="N32" s="1">
+        <v>19</v>
+      </c>
+      <c r="O32" s="1">
+        <v>14</v>
+      </c>
+      <c r="P32" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>17</v>
+      </c>
+      <c r="R32" s="1">
+        <v>10</v>
+      </c>
+      <c r="S32" s="1">
+        <v>9</v>
+      </c>
+      <c r="T32" s="1">
+        <v>5</v>
+      </c>
+      <c r="U32" s="1">
+        <v>8</v>
+      </c>
+      <c r="V32" s="1">
+        <v>4</v>
+      </c>
+      <c r="W32" s="1">
+        <v>3</v>
+      </c>
+      <c r="X32" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y32" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z32" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>13</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC32" s="1">
+        <f>SUM(B32:AB32)</f>
+        <v>287</v>
+      </c>
+      <c r="AD32" s="9">
+        <f>SUM(B32:AB32)/27</f>
+        <v>10.62962962962963</v>
+      </c>
+      <c r="AE32" s="9">
+        <f>_xlfn.STDEV.S(B32:AB32)</f>
+        <v>5.4218088675285658</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
+        <v>21</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <v>10</v>
+      </c>
+      <c r="D33" s="2">
+        <v>5</v>
+      </c>
+      <c r="E33" s="1">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1">
+        <v>10</v>
+      </c>
+      <c r="G33" s="1">
+        <v>11</v>
+      </c>
+      <c r="H33" s="1">
+        <v>18</v>
+      </c>
+      <c r="I33" s="1">
+        <v>17</v>
+      </c>
+      <c r="J33" s="1">
+        <v>23</v>
+      </c>
+      <c r="K33" s="1">
+        <v>13</v>
+      </c>
+      <c r="L33" s="1">
+        <v>9</v>
+      </c>
+      <c r="M33" s="1">
+        <v>19</v>
+      </c>
+      <c r="N33" s="1">
+        <v>16</v>
+      </c>
+      <c r="O33" s="1">
+        <v>19</v>
+      </c>
+      <c r="P33" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>17</v>
+      </c>
+      <c r="R33" s="1">
+        <v>6</v>
+      </c>
+      <c r="S33" s="1">
+        <v>8</v>
+      </c>
+      <c r="T33" s="1">
+        <v>9</v>
+      </c>
+      <c r="U33" s="1">
+        <v>5</v>
+      </c>
+      <c r="V33" s="1">
+        <v>10</v>
+      </c>
+      <c r="W33" s="1">
+        <v>11</v>
+      </c>
+      <c r="X33" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC33" s="1">
+        <f>SUM(B33:AB33)</f>
+        <v>289</v>
+      </c>
+      <c r="AD33" s="9">
+        <f>SUM(B33:AB33)/27</f>
+        <v>10.703703703703704</v>
+      </c>
+      <c r="AE33" s="9">
+        <f>_xlfn.STDEV.S(B33:AB33)</f>
+        <v>5.4759250347092028</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12">
+        <v>5</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>9</v>
+      </c>
+      <c r="D34" s="2">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1">
+        <v>19</v>
+      </c>
+      <c r="F34" s="1">
+        <v>18</v>
+      </c>
+      <c r="G34" s="1">
+        <v>10</v>
+      </c>
+      <c r="H34" s="1">
+        <v>9</v>
+      </c>
+      <c r="I34" s="1">
+        <v>15</v>
+      </c>
+      <c r="J34" s="1">
+        <v>11</v>
+      </c>
+      <c r="K34" s="1">
+        <v>22</v>
+      </c>
+      <c r="L34" s="1">
+        <v>20</v>
+      </c>
+      <c r="M34" s="1">
+        <v>14</v>
+      </c>
+      <c r="N34" s="1">
+        <v>14</v>
+      </c>
+      <c r="O34" s="1">
+        <v>10</v>
+      </c>
+      <c r="P34" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>18</v>
+      </c>
+      <c r="R34" s="1">
+        <v>11</v>
+      </c>
+      <c r="S34" s="1">
+        <v>7</v>
+      </c>
+      <c r="T34" s="1">
+        <v>7</v>
+      </c>
+      <c r="U34" s="1">
+        <v>5</v>
+      </c>
+      <c r="V34" s="1">
+        <v>8</v>
+      </c>
+      <c r="W34" s="1">
+        <v>4</v>
+      </c>
+      <c r="X34" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y34" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z34" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA34" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="1">
+        <f>SUM(B34:AB34)</f>
+        <v>287</v>
+      </c>
+      <c r="AD34" s="9">
+        <f>SUM(B34:AB34)/27</f>
+        <v>10.62962962962963</v>
+      </c>
+      <c r="AE34" s="9">
+        <f>_xlfn.STDEV.S(B34:AB34)</f>
+        <v>5.5062771741974919</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
+        <v>13</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2">
+        <v>15</v>
+      </c>
+      <c r="D35" s="2">
+        <v>9</v>
+      </c>
+      <c r="E35" s="1">
+        <v>19</v>
+      </c>
+      <c r="F35" s="1">
+        <v>13</v>
+      </c>
+      <c r="G35" s="1">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1">
+        <v>11</v>
+      </c>
+      <c r="I35" s="1">
+        <v>19</v>
+      </c>
+      <c r="J35" s="1">
+        <v>10</v>
+      </c>
+      <c r="K35" s="1">
+        <v>19</v>
+      </c>
+      <c r="L35" s="1">
+        <v>16</v>
+      </c>
+      <c r="M35" s="1">
+        <v>15</v>
+      </c>
+      <c r="N35" s="1">
+        <v>17</v>
+      </c>
+      <c r="O35" s="1">
+        <v>24</v>
+      </c>
+      <c r="P35" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>13</v>
+      </c>
+      <c r="R35" s="1">
+        <v>7</v>
+      </c>
+      <c r="S35" s="1">
+        <v>11</v>
+      </c>
+      <c r="T35" s="1">
+        <v>6</v>
+      </c>
+      <c r="U35" s="1">
+        <v>5</v>
+      </c>
+      <c r="V35" s="1">
+        <v>7</v>
+      </c>
+      <c r="W35" s="1">
+        <v>8</v>
+      </c>
+      <c r="X35" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z35" s="1">
+        <v>13</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC35" s="1">
+        <f>SUM(B35:AB35)</f>
+        <v>317</v>
+      </c>
+      <c r="AD35" s="9">
+        <f>SUM(B35:AB35)/27</f>
+        <v>11.74074074074074</v>
+      </c>
+      <c r="AE35" s="9">
+        <f>_xlfn.STDEV.S(B35:AB35)</f>
+        <v>5.5580336353550335</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="15">
+        <v>22</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>9</v>
+      </c>
+      <c r="D36" s="2">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1">
+        <v>19</v>
+      </c>
+      <c r="F36" s="1">
+        <v>12</v>
+      </c>
+      <c r="G36" s="1">
+        <v>16</v>
+      </c>
+      <c r="H36" s="1">
+        <v>15</v>
+      </c>
+      <c r="I36" s="1">
+        <v>16</v>
+      </c>
+      <c r="J36" s="1">
+        <v>11</v>
+      </c>
+      <c r="K36" s="1">
+        <v>18</v>
+      </c>
+      <c r="L36" s="1">
+        <v>20</v>
+      </c>
+      <c r="M36" s="1">
+        <v>14</v>
+      </c>
+      <c r="N36" s="1">
+        <v>20</v>
+      </c>
+      <c r="O36" s="1">
+        <v>16</v>
+      </c>
+      <c r="P36" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>12</v>
+      </c>
+      <c r="R36" s="1">
+        <v>13</v>
+      </c>
+      <c r="S36" s="1">
+        <v>8</v>
+      </c>
+      <c r="T36" s="1">
+        <v>5</v>
+      </c>
+      <c r="U36" s="1">
+        <v>2</v>
+      </c>
+      <c r="V36" s="1">
+        <v>5</v>
+      </c>
+      <c r="W36" s="1">
+        <v>9</v>
+      </c>
+      <c r="X36" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y36" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z36" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA36" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="1">
+        <f>SUM(B36:AB36)</f>
+        <v>290</v>
+      </c>
+      <c r="AD36" s="9">
+        <f>SUM(B36:AB36)/27</f>
+        <v>10.74074074074074</v>
+      </c>
+      <c r="AE36" s="9">
+        <f>_xlfn.STDEV.S(B36:AB36)</f>
+        <v>5.7015017764728011</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="18">
+        <v>42</v>
+      </c>
+      <c r="B37" s="2">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2">
+        <v>8</v>
+      </c>
+      <c r="D37" s="2">
+        <v>5</v>
+      </c>
+      <c r="E37" s="1">
+        <v>13</v>
+      </c>
+      <c r="F37" s="1">
+        <v>19</v>
+      </c>
+      <c r="G37" s="1">
+        <v>16</v>
+      </c>
+      <c r="H37" s="1">
+        <v>20</v>
+      </c>
+      <c r="I37" s="1">
+        <v>10</v>
+      </c>
+      <c r="J37" s="1">
+        <v>13</v>
+      </c>
+      <c r="K37" s="1">
+        <v>14</v>
+      </c>
+      <c r="L37" s="1">
+        <v>13</v>
+      </c>
+      <c r="M37" s="1">
+        <v>17</v>
+      </c>
+      <c r="N37" s="1">
+        <v>9</v>
+      </c>
+      <c r="O37" s="1">
+        <v>14</v>
+      </c>
+      <c r="P37" s="1">
+        <v>17</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>11</v>
+      </c>
+      <c r="R37" s="1">
+        <v>13</v>
+      </c>
+      <c r="S37" s="1">
+        <v>8</v>
+      </c>
+      <c r="T37" s="1">
+        <v>13</v>
+      </c>
+      <c r="U37" s="1">
+        <v>9</v>
+      </c>
+      <c r="V37" s="1">
+        <v>8</v>
+      </c>
+      <c r="W37" s="1">
+        <v>5</v>
+      </c>
+      <c r="X37" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="1">
+        <f>SUM(B37:AB37)</f>
+        <v>265</v>
+      </c>
+      <c r="AD37" s="9">
+        <f>SUM(B37:AB37)/27</f>
+        <v>9.8148148148148149</v>
+      </c>
+      <c r="AE37" s="9">
+        <f>_xlfn.STDEV.S(B37:AB37)</f>
+        <v>5.9293081516054764</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="16">
+        <v>34</v>
+      </c>
+      <c r="B38" s="2">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2">
+        <v>12</v>
+      </c>
+      <c r="D38" s="2">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1">
+        <v>14</v>
+      </c>
+      <c r="F38" s="1">
+        <v>20</v>
+      </c>
+      <c r="G38" s="1">
+        <v>25</v>
+      </c>
+      <c r="H38" s="1">
+        <v>12</v>
+      </c>
+      <c r="I38" s="1">
+        <v>20</v>
+      </c>
+      <c r="J38" s="1">
+        <v>13</v>
+      </c>
+      <c r="K38" s="1">
+        <v>12</v>
+      </c>
+      <c r="L38" s="1">
+        <v>10</v>
+      </c>
+      <c r="M38" s="1">
+        <v>9</v>
+      </c>
+      <c r="N38" s="1">
+        <v>17</v>
+      </c>
+      <c r="O38" s="1">
+        <v>12</v>
+      </c>
+      <c r="P38" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>16</v>
+      </c>
+      <c r="R38" s="1">
+        <v>14</v>
+      </c>
+      <c r="S38" s="1">
+        <v>5</v>
+      </c>
+      <c r="T38" s="1">
+        <v>4</v>
+      </c>
+      <c r="U38" s="1">
+        <v>4</v>
+      </c>
+      <c r="V38" s="1">
+        <v>4</v>
+      </c>
+      <c r="W38" s="1">
+        <v>10</v>
+      </c>
+      <c r="X38" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y38" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA38" s="1">
+        <v>8</v>
+      </c>
+      <c r="AB38" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC38" s="1">
+        <f>SUM(B38:AB38)</f>
+        <v>291</v>
+      </c>
+      <c r="AD38" s="9">
+        <f>SUM(B38:AB38)/27</f>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="AE38" s="9">
+        <f>_xlfn.STDEV.S(B38:AB38)</f>
+        <v>5.9312298201542637</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
+        <v>39</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>14</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2</v>
+      </c>
+      <c r="E39" s="1">
+        <v>10</v>
+      </c>
+      <c r="F39" s="1">
+        <v>11</v>
+      </c>
+      <c r="G39" s="1">
+        <v>13</v>
+      </c>
+      <c r="H39" s="1">
+        <v>16</v>
+      </c>
+      <c r="I39" s="1">
+        <v>14</v>
+      </c>
+      <c r="J39" s="1">
+        <v>7</v>
+      </c>
+      <c r="K39" s="1">
+        <v>14</v>
+      </c>
+      <c r="L39" s="1">
+        <v>12</v>
+      </c>
+      <c r="M39" s="1">
+        <v>14</v>
+      </c>
+      <c r="N39" s="1">
+        <v>18</v>
+      </c>
+      <c r="O39" s="1">
+        <v>16</v>
+      </c>
+      <c r="P39" s="1">
+        <v>22</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>8</v>
+      </c>
+      <c r="R39" s="1">
+        <v>13</v>
+      </c>
+      <c r="S39" s="1">
+        <v>6</v>
+      </c>
+      <c r="T39" s="1">
+        <v>11</v>
+      </c>
+      <c r="U39" s="1">
+        <v>12</v>
+      </c>
+      <c r="V39" s="1">
+        <v>13</v>
+      </c>
+      <c r="W39" s="1">
+        <v>7</v>
+      </c>
+      <c r="X39" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y39" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="1">
+        <f>SUM(B39:AB39)</f>
+        <v>264</v>
+      </c>
+      <c r="AD39" s="9">
+        <f>SUM(B39:AB39)/27</f>
+        <v>9.7777777777777786</v>
+      </c>
+      <c r="AE39" s="9">
+        <f>_xlfn.STDEV.S(B39:AB39)</f>
+        <v>5.9571116732171037</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14">
+        <v>12</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2">
+        <v>15</v>
+      </c>
+      <c r="D40" s="2">
+        <v>7</v>
+      </c>
+      <c r="E40" s="1">
+        <v>10</v>
+      </c>
+      <c r="F40" s="1">
+        <v>12</v>
+      </c>
+      <c r="G40" s="1">
+        <v>19</v>
+      </c>
+      <c r="H40" s="1">
+        <v>11</v>
+      </c>
+      <c r="I40" s="1">
+        <v>12</v>
+      </c>
+      <c r="J40" s="1">
+        <v>22</v>
+      </c>
+      <c r="K40" s="1">
+        <v>19</v>
+      </c>
+      <c r="L40" s="1">
+        <v>17</v>
+      </c>
+      <c r="M40" s="1">
+        <v>19</v>
+      </c>
+      <c r="N40" s="1">
+        <v>15</v>
+      </c>
+      <c r="O40" s="1">
+        <v>11</v>
+      </c>
+      <c r="P40" s="1">
+        <v>17</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>19</v>
+      </c>
+      <c r="R40" s="1">
+        <v>15</v>
+      </c>
+      <c r="S40" s="1">
+        <v>4</v>
+      </c>
+      <c r="T40" s="1">
+        <v>4</v>
+      </c>
+      <c r="U40" s="1">
+        <v>6</v>
+      </c>
+      <c r="V40" s="1">
+        <v>11</v>
+      </c>
+      <c r="W40" s="1">
+        <v>5</v>
+      </c>
+      <c r="X40" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y40" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z40" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA40" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB40" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC40" s="1">
+        <f>SUM(B40:AB40)</f>
+        <v>302</v>
+      </c>
+      <c r="AD40" s="9">
+        <f>SUM(B40:AB40)/27</f>
+        <v>11.185185185185185</v>
+      </c>
+      <c r="AE40" s="9">
+        <f>_xlfn.STDEV.S(B40:AB40)</f>
+        <v>6.0066439947588099</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17">
+        <v>41</v>
+      </c>
+      <c r="B41" s="8">
+        <v>1</v>
+      </c>
+      <c r="C41" s="8">
+        <v>23</v>
+      </c>
+      <c r="D41" s="8">
+        <v>10</v>
+      </c>
+      <c r="E41" s="7">
+        <v>13</v>
+      </c>
+      <c r="F41" s="7">
+        <v>13</v>
+      </c>
+      <c r="G41" s="7">
+        <v>14</v>
+      </c>
+      <c r="H41" s="7">
+        <v>11</v>
+      </c>
+      <c r="I41" s="7">
+        <v>12</v>
+      </c>
+      <c r="J41" s="7">
+        <v>14</v>
+      </c>
+      <c r="K41" s="7">
+        <v>15</v>
+      </c>
+      <c r="L41" s="7">
+        <v>7</v>
+      </c>
+      <c r="M41" s="7">
+        <v>10</v>
+      </c>
+      <c r="N41" s="7">
+        <v>6</v>
+      </c>
+      <c r="O41" s="7">
+        <v>14</v>
+      </c>
+      <c r="P41" s="7">
+        <v>16</v>
+      </c>
+      <c r="Q41" s="7">
+        <v>15</v>
+      </c>
+      <c r="R41" s="7">
+        <v>15</v>
+      </c>
+      <c r="S41" s="7">
+        <v>13</v>
+      </c>
+      <c r="T41" s="7">
+        <v>8</v>
+      </c>
+      <c r="U41" s="7">
+        <v>3</v>
+      </c>
+      <c r="V41" s="7">
+        <v>7</v>
+      </c>
+      <c r="W41" s="7">
+        <v>8</v>
+      </c>
+      <c r="X41" s="7">
+        <v>6</v>
+      </c>
+      <c r="Y41" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="7">
+        <f>SUM(B41:AB41)</f>
+        <v>254</v>
+      </c>
+      <c r="AD41" s="9">
+        <f>SUM(B41:AB41)/27</f>
+        <v>9.4074074074074066</v>
+      </c>
+      <c r="AE41" s="9">
+        <f>_xlfn.STDEV.S(B41:AB41)</f>
+        <v>6.0080667520314801</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="16">
+        <v>37</v>
+      </c>
+      <c r="B42" s="2">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2">
+        <v>16</v>
+      </c>
+      <c r="D42" s="2">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1">
+        <v>13</v>
+      </c>
+      <c r="F42" s="1">
+        <v>10</v>
+      </c>
+      <c r="G42" s="1">
+        <v>11</v>
+      </c>
+      <c r="H42" s="1">
+        <v>18</v>
+      </c>
+      <c r="I42" s="1">
+        <v>15</v>
+      </c>
+      <c r="J42" s="1">
+        <v>9</v>
+      </c>
+      <c r="K42" s="1">
+        <v>16</v>
+      </c>
+      <c r="L42" s="1">
+        <v>17</v>
+      </c>
+      <c r="M42" s="1">
+        <v>12</v>
+      </c>
+      <c r="N42" s="1">
+        <v>16</v>
+      </c>
+      <c r="O42" s="1">
+        <v>16</v>
+      </c>
+      <c r="P42" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>19</v>
+      </c>
+      <c r="R42" s="1">
+        <v>15</v>
+      </c>
+      <c r="S42" s="1">
+        <v>5</v>
+      </c>
+      <c r="T42" s="1">
+        <v>4</v>
+      </c>
+      <c r="U42" s="1">
+        <v>7</v>
+      </c>
+      <c r="V42" s="1">
+        <v>5</v>
+      </c>
+      <c r="W42" s="1">
+        <v>6</v>
+      </c>
+      <c r="X42" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y42" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z42" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="1">
+        <f>SUM(B42:AB42)</f>
+        <v>260</v>
+      </c>
+      <c r="AD42" s="9">
+        <f>SUM(B42:AB42)/27</f>
+        <v>9.6296296296296298</v>
+      </c>
+      <c r="AE42" s="9">
+        <f>_xlfn.STDEV.S(B42:AB42)</f>
+        <v>6.0265320308688572</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="18">
+        <v>40</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>17</v>
+      </c>
+      <c r="D43" s="2">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1">
+        <v>7</v>
+      </c>
+      <c r="F43" s="1">
+        <v>11</v>
+      </c>
+      <c r="G43" s="1">
+        <v>19</v>
+      </c>
+      <c r="H43" s="1">
+        <v>19</v>
+      </c>
+      <c r="I43" s="1">
+        <v>13</v>
+      </c>
+      <c r="J43" s="1">
+        <v>9</v>
+      </c>
+      <c r="K43" s="1">
+        <v>13</v>
+      </c>
+      <c r="L43" s="1">
+        <v>12</v>
+      </c>
+      <c r="M43" s="1">
+        <v>18</v>
+      </c>
+      <c r="N43" s="1">
+        <v>15</v>
+      </c>
+      <c r="O43" s="1">
+        <v>9</v>
+      </c>
+      <c r="P43" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>17</v>
+      </c>
+      <c r="R43" s="1">
+        <v>12</v>
+      </c>
+      <c r="S43" s="1">
+        <v>11</v>
+      </c>
+      <c r="T43" s="1">
+        <v>6</v>
+      </c>
+      <c r="U43" s="1">
+        <v>10</v>
+      </c>
+      <c r="V43" s="1">
+        <v>6</v>
+      </c>
+      <c r="W43" s="1">
+        <v>6</v>
+      </c>
+      <c r="X43" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="1">
+        <f>SUM(B43:AB43)</f>
+        <v>254</v>
+      </c>
+      <c r="AD43" s="9">
+        <f>SUM(B43:AB43)/27</f>
+        <v>9.4074074074074066</v>
+      </c>
+      <c r="AE43" s="9">
+        <f>_xlfn.STDEV.S(B43:AB43)</f>
+        <v>6.0717457840473585</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2">
+        <v>2</v>
+      </c>
+      <c r="C44" s="2">
+        <v>14</v>
+      </c>
+      <c r="D44" s="2">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1">
+        <v>18</v>
+      </c>
+      <c r="F44" s="1">
+        <v>18</v>
+      </c>
+      <c r="G44" s="1">
+        <v>12</v>
+      </c>
+      <c r="H44" s="1">
+        <v>11</v>
+      </c>
+      <c r="I44" s="1">
+        <v>19</v>
+      </c>
+      <c r="J44" s="1">
+        <v>14</v>
+      </c>
+      <c r="K44" s="1">
+        <v>10</v>
+      </c>
+      <c r="L44" s="1">
+        <v>8</v>
+      </c>
+      <c r="M44" s="1">
+        <v>19</v>
+      </c>
+      <c r="N44" s="1">
+        <v>17</v>
+      </c>
+      <c r="O44" s="1">
+        <v>12</v>
+      </c>
+      <c r="P44" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>10</v>
+      </c>
+      <c r="R44" s="1">
+        <v>13</v>
+      </c>
+      <c r="S44" s="1">
+        <v>9</v>
+      </c>
+      <c r="T44" s="1">
+        <v>12</v>
+      </c>
+      <c r="U44" s="1">
+        <v>6</v>
+      </c>
+      <c r="V44" s="1">
+        <v>8</v>
+      </c>
+      <c r="W44" s="1">
+        <v>8</v>
+      </c>
+      <c r="X44" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="1">
+        <f>SUM(B44:AB44)</f>
+        <v>268</v>
+      </c>
+      <c r="AD44" s="9">
+        <f>SUM(B44:AB44)/27</f>
+        <v>9.9259259259259256</v>
+      </c>
+      <c r="AE44" s="9">
+        <f>_xlfn.STDEV.S(B44:AB44)</f>
+        <v>6.2260366818332153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="18">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0</v>
+      </c>
+      <c r="C45" s="2">
+        <v>15</v>
+      </c>
+      <c r="D45" s="2">
+        <v>10</v>
+      </c>
+      <c r="E45" s="1">
+        <v>18</v>
+      </c>
+      <c r="F45" s="1">
+        <v>10</v>
+      </c>
+      <c r="G45" s="1">
+        <v>13</v>
+      </c>
+      <c r="H45" s="1">
+        <v>10</v>
+      </c>
+      <c r="I45" s="1">
+        <v>19</v>
+      </c>
+      <c r="J45" s="1">
+        <v>17</v>
+      </c>
+      <c r="K45" s="1">
+        <v>6</v>
+      </c>
+      <c r="L45" s="1">
+        <v>18</v>
+      </c>
+      <c r="M45" s="1">
+        <v>16</v>
+      </c>
+      <c r="N45" s="1">
+        <v>14</v>
+      </c>
+      <c r="O45" s="1">
+        <v>10</v>
+      </c>
+      <c r="P45" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>12</v>
+      </c>
+      <c r="R45" s="1">
+        <v>9</v>
+      </c>
+      <c r="S45" s="1">
+        <v>3</v>
+      </c>
+      <c r="T45" s="1">
+        <v>5</v>
+      </c>
+      <c r="U45" s="1">
+        <v>10</v>
+      </c>
+      <c r="V45" s="1">
+        <v>4</v>
+      </c>
+      <c r="W45" s="1">
+        <v>0</v>
+      </c>
+      <c r="X45" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="1">
+        <f>SUM(B45:AB45)</f>
+        <v>231</v>
+      </c>
+      <c r="AD45" s="9">
+        <f>SUM(B45:AB45)/27</f>
+        <v>8.5555555555555554</v>
+      </c>
+      <c r="AE45" s="9">
+        <f>_xlfn.STDEV.S(B45:AB45)</f>
+        <v>6.5711100416510435</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4">
+        <v>2</v>
+      </c>
+      <c r="C46" s="4">
+        <v>15</v>
+      </c>
+      <c r="D46" s="4">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3">
+        <v>15</v>
+      </c>
+      <c r="F46" s="3">
+        <v>23</v>
+      </c>
+      <c r="G46" s="3">
+        <v>14</v>
+      </c>
+      <c r="H46" s="3">
+        <v>9</v>
+      </c>
+      <c r="I46" s="3">
+        <v>15</v>
+      </c>
+      <c r="J46" s="3">
+        <v>11</v>
+      </c>
+      <c r="K46" s="3">
+        <v>18</v>
+      </c>
+      <c r="L46" s="3">
+        <v>13</v>
+      </c>
+      <c r="M46" s="3">
+        <v>14</v>
+      </c>
+      <c r="N46" s="3">
+        <v>13</v>
+      </c>
+      <c r="O46" s="3">
+        <v>13</v>
+      </c>
+      <c r="P46" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>18</v>
+      </c>
+      <c r="R46" s="3">
+        <v>15</v>
+      </c>
+      <c r="S46" s="3">
+        <v>5</v>
+      </c>
+      <c r="T46" s="3">
+        <v>10</v>
+      </c>
+      <c r="U46" s="3">
+        <v>12</v>
+      </c>
+      <c r="V46" s="3">
+        <v>8</v>
+      </c>
+      <c r="W46" s="3">
+        <v>0</v>
+      </c>
+      <c r="X46" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="3">
+        <f>SUM(B46:AB46)</f>
+        <v>266</v>
+      </c>
+      <c r="AD46" s="9">
+        <f>SUM(B46:AB46)/27</f>
+        <v>9.8518518518518512</v>
+      </c>
+      <c r="AE46" s="9">
+        <f>_xlfn.STDEV.S(B46:AB46)</f>
+        <v>6.7465301834105444</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AE1">
+    <sortState ref="A2:AE46">
+      <sortCondition ref="AE1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>